<commit_message>
"like a pro" article added
</commit_message>
<xml_diff>
--- a/private/socialmedia_follower_tracker.xlsx
+++ b/private/socialmedia_follower_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\lolvvv1\private\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B832C175-4445-4FC7-8560-71859C83F5D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCFBDD1-3248-4008-98C8-19B5D528A760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3675" windowWidth="29040" windowHeight="15840" xr2:uid="{CD54439B-FD1D-4D5B-A9F3-2CED96D4A811}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{CD54439B-FD1D-4D5B-A9F3-2CED96D4A811}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -410,52 +410,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF8A31A-E7DE-4A63-B50C-67C6F17AD800}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
         <v>44174</v>
       </c>
+      <c r="C1" s="2">
+        <v>44186</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>330</v>
       </c>
+      <c r="C2">
+        <v>328</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>458</v>
       </c>
+      <c r="C3">
+        <v>458</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>924</v>
       </c>
+      <c r="C4">
+        <v>941</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>36</v>
+      </c>
+      <c r="C5">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>